<commit_message>
Finished version more music
</commit_message>
<xml_diff>
--- a/resources/stroop.xlsx
+++ b/resources/stroop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carelab\Desktop\Erik\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A848CC-F990-473B-9DBA-E18ACF5EAFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B8A9DB-C1DF-4A74-80AA-03908638AF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7541B1D4-D6BA-4590-87FC-BB33B7C796A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7541B1D4-D6BA-4590-87FC-BB33B7C796A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="16">
   <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
     <t>red</t>
   </si>
   <si>
@@ -63,12 +57,6 @@
     <t>correct</t>
   </si>
   <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>YELLOW</t>
-  </si>
-  <si>
     <t>yellow</t>
   </si>
   <si>
@@ -82,6 +70,18 @@
   </si>
   <si>
     <t>rand</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>RED</t>
   </si>
 </sst>
 </file>
@@ -435,1104 +435,1104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E624250-F574-4026-BB3C-4589944587B5}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D65" ca="1" si="0">RAND()</f>
-        <v>0.66145458981333727</v>
+        <v>9.3144791325373899E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8128958267552191</v>
+        <v>0.45281526645097336</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43264577324607045</v>
+        <v>0.17809999888779438</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27604298475476152</v>
+        <v>0.61493103085715994</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28788112805048449</v>
+        <v>0.87103612147153631</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25688780612826978</v>
+        <v>0.1436934197931079</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3962155004358756E-2</v>
+        <v>0.28723437633798032</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16149260709460955</v>
+        <v>0.73449052989125296</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94283827128599695</v>
+        <v>0.72210065569241355</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87762360501245729</v>
+        <v>0.79383620601823524</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34192124773831323</v>
+        <v>0.87025490562902552</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11961469589149154</v>
+        <v>0.98698650967505908</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47768273959416241</v>
+        <v>0.5540108446021621</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7132979650671998E-2</v>
+        <v>0.10226013230401498</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2372052746712412</v>
+        <v>0.7326194956219807</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81313056186010058</v>
+        <v>0.70064692691216712</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20644192159915542</v>
+        <v>0.56312153978378932</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79723106747808248</v>
+        <v>0.6007167790447655</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80030098005232186</v>
+        <v>0.5333334761316173</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13077210193367239</v>
+        <v>0.11646385491494626</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44101927638488736</v>
+        <v>0.74669229220719535</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29508985178613967</v>
+        <v>0.85777311605750339</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80684954756871874</v>
+        <v>0.83543545754873827</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85485853519045751</v>
+        <v>0.34446592250373875</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96472937093937816</v>
+        <v>0.51834127987047374</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>1.118403874071372E-2</v>
+        <v>0.19240256530656463</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63690338159864524</v>
+        <v>0.16787133307814683</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89957407334590633</v>
+        <v>0.21078651124033343</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
         <v>3</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89126478050659985</v>
+        <v>0.82461097485288803</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52981334304736982</v>
+        <v>0.18793391056818876</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56743317093431245</v>
+        <v>0.69455994901692264</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>6.591400966360883E-2</v>
+        <v>0.89367785291182467</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21192191501919622</v>
+        <v>7.3213309436405583E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88903570707608381</v>
+        <v>0.93496244219991342</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6920070545067287E-2</v>
+        <v>0.47024875746249362</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96622926717906243</v>
+        <v>0.1006635488895874</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6103908603094943</v>
+        <v>0.19051325419023346</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48472373821132564</v>
+        <v>0.52652642987719556</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.660253953015428</v>
+        <v>0.56862685120773782</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38248203776335621</v>
+        <v>0.23206704470430572</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="0"/>
-        <v>2.700978295652301E-2</v>
+        <v>4.5288053640182513E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86698835379248962</v>
+        <v>0.43080741715641402</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23924239463121821</v>
+        <v>0.18799302094368442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
         <v>3</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
       <c r="D45">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62613403564832892</v>
+        <v>0.2269112088478803</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53660567572501527</v>
+        <v>0.92789171017784489</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>3</v>
       </c>
-      <c r="C47" t="s">
-        <v>5</v>
-      </c>
       <c r="D47">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9926552134725539E-2</v>
+        <v>0.24287166306265751</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
         <v>3</v>
       </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
       <c r="D48">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87978102521483792</v>
+        <v>0.6527343509422131</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3574410811547245</v>
+        <v>0.55792239260830501</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70626745422902226</v>
+        <v>0.4009422111305545</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15603936871830648</v>
+        <v>0.22008998513319111</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87303922084863261</v>
+        <v>0.71467323886249834</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
         <v>1</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>3</v>
       </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
       <c r="D53">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46870002227673579</v>
+        <v>0.45209603025284606</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4075324863091865E-2</v>
+        <v>7.3616507322166846E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76063852046492852</v>
+        <v>0.27111647240318137</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
         <v>1</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>3</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
       <c r="D56">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16717878746525761</v>
+        <v>0.81172391986647774</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79602967754943599</v>
+        <v>0.40817250924350401</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50313400742600822</v>
+        <v>0.33296037424380831</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52068852235734386</v>
+        <v>9.4262782491351227E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77913546310317416</v>
+        <v>0.84357197633087588</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57028643313919924</v>
+        <v>0.44028386888225768</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
         <v>3</v>
       </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
       <c r="D62">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72866109517460265</v>
+        <v>0.19795486748994306</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
         <v>3</v>
       </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
       <c r="D63">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79669299437701868</v>
+        <v>0.60755433258693681</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27958214679197679</v>
+        <v>0.9862391246911979</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
         <v>9</v>
       </c>
-      <c r="B65" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" t="s">
-        <v>13</v>
-      </c>
       <c r="D65">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89220099478138126</v>
+        <v>0.21700233089842735</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
         <v>3</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
       </c>
       <c r="D66">
         <f t="shared" ref="D66:D73" ca="1" si="1">RAND()</f>
-        <v>0.51161359094010417</v>
+        <v>0.46316559430037219</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16317623495334865</v>
+        <v>0.25592210451755715</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86643535926267445</v>
+        <v>0.22405821601442855</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6620941506003017E-2</v>
+        <v>0.83303894603955364</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71209835503321106</v>
+        <v>0.57825691074150742</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72668794399742132</v>
+        <v>0.84744460889134443</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17439998922396605</v>
+        <v>0.80318762675704003</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14027814160498253</v>
+        <v>0.62305632447745951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>